<commit_message>
First complete version project 5.
</commit_message>
<xml_diff>
--- a/5_IdentifyFraudFromEnronEmail/final_project/Project 5 stats.xlsx
+++ b/5_IdentifyFraudFromEnronEmail/final_project/Project 5 stats.xlsx
@@ -9,12 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="5475" windowHeight="4665"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="5475" windowHeight="4665" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId2"/>
-    <sheet name="Correlation" sheetId="3" r:id="rId3"/>
+    <sheet name="Correlation" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -206,7 +205,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="178" formatCode="0.000_ "/>
+    <numFmt numFmtId="176" formatCode="0.000_ "/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -290,19 +289,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
@@ -601,7 +600,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -804,25 +803,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.375" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>